<commit_message>
mengedit isi dataset XBR_USD.xlsx
</commit_message>
<xml_diff>
--- a/Preprocess Logam dan Minyak/XBR_USD.xlsx
+++ b/Preprocess Logam dan Minyak/XBR_USD.xlsx
@@ -9293,7 +9293,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -9781,7 +9781,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10141,8 +10141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A980" workbookViewId="0">
+      <selection activeCell="A989" sqref="A989"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>